<commit_message>
patch sur le format des données
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION6.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8795AC-5C54-4E6A-867B-B20F40A02ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9B175-C2B2-4444-9096-9F28A71F77D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -347,9 +347,6 @@
     <t>TOTAL COMPATIBLE</t>
   </si>
   <si>
-    <t xml:space="preserve">Objectif : 70 % </t>
-  </si>
-  <si>
     <t>NON</t>
   </si>
   <si>
@@ -360,6 +357,33 @@
   </si>
   <si>
     <t>9m40</t>
+  </si>
+  <si>
+    <t>22m08</t>
+  </si>
+  <si>
+    <t>6m22</t>
+  </si>
+  <si>
+    <t>3m48</t>
+  </si>
+  <si>
+    <t>13s</t>
+  </si>
+  <si>
+    <t>30m10</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMENTAIRE </t>
+  </si>
+  <si>
+    <t>LA FAMILLE CV4 DOIT ETRE SUPPRIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIX NET </t>
   </si>
 </sst>
 </file>
@@ -729,10 +753,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,11 +766,12 @@
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,16 +782,20 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -776,11 +805,14 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
       <c r="E2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -790,11 +822,14 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
       <c r="E3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -804,11 +839,17 @@
       <c r="C4" t="s">
         <v>82</v>
       </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
       <c r="E4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -822,7 +863,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -832,11 +873,14 @@
       <c r="C6" t="s">
         <v>40</v>
       </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
       <c r="E6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -850,7 +894,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -860,11 +904,17 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
       <c r="E8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -874,11 +924,14 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
       <c r="E9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -892,7 +945,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -903,10 +956,10 @@
         <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -916,11 +969,14 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -934,7 +990,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -948,7 +1004,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -962,7 +1018,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -976,7 +1032,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -990,7 +1046,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1004,24 +1060,24 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1035,7 +1091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1049,7 +1105,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1062,15 +1118,13 @@
       <c r="E22" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="4" t="str">
+      <c r="G22" s="4" t="str">
         <f>"Total : " &amp;ROUND(COUNTIF(E:E,"OUI")/53*100,2) &amp; "%"</f>
-        <v>Total : 86,79%</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>Total : 90,57%</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1083,12 +1137,13 @@
       <c r="E23" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="4" t="str">
+      <c r="G23" s="4" t="str">
         <f>"Nombre incompatible : " &amp;COUNTIF(E2:E54,"NON")</f>
-        <v>Nombre incompatible : 7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>Nombre incompatible : 5</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1098,15 +1153,19 @@
       <c r="C24" t="s">
         <v>47</v>
       </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
       <c r="E24" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="4" t="str">
+      <c r="G24" s="4" t="str">
         <f>"Total incompatible : " &amp;ROUND(COUNTIF(E:E,"NON")/53*100,2) &amp; "%"</f>
-        <v>Total incompatible : 13,21%</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>Total incompatible : 9,43%</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1120,7 +1179,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1134,7 +1193,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1144,11 +1203,14 @@
       <c r="C27" t="s">
         <v>65</v>
       </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
       <c r="E27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1224,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1238,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1252,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1204,7 +1266,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1354,8 +1416,11 @@
       <c r="C42" t="s">
         <v>44</v>
       </c>
+      <c r="D42" t="s">
+        <v>112</v>
+      </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,8 +1447,11 @@
       <c r="C44" t="s">
         <v>21</v>
       </c>
+      <c r="D44" t="s">
+        <v>112</v>
+      </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,7 +1577,7 @@
         <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,10 +1596,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A54" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H54">
     <sortCondition ref="A2:A54"/>
   </sortState>
-  <conditionalFormatting sqref="F1 G21 F22 E1:E1048576">
+  <conditionalFormatting sqref="G1:H1 G22:H22 E1:F4 E6:F1048576 E5">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NON">
       <formula>NOT(ISERROR(SEARCH("NON",E1)))</formula>
     </cfRule>
@@ -1540,7 +1608,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
probleme de format dans tarificator lors de la comparaison du RVAL avec 0,01
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9B175-C2B2-4444-9096-9F28A71F77D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3EEE0F-4452-4C6A-9E30-A21B04A1464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="117">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t xml:space="preserve">PRIX NET </t>
+  </si>
+  <si>
+    <t>9m30</t>
   </si>
 </sst>
 </file>
@@ -755,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,6 +1466,9 @@
       </c>
       <c r="C45" t="s">
         <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
       </c>
       <c r="E45" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Tarificator : Ajout d'un filtre qui empeche un utilisateur de lancer un tarif qui n'est pas compatible.
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3EEE0F-4452-4C6A-9E30-A21B04A1464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66CAC91-6541-412F-A312-F0ED194D6A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="117">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -338,9 +338,6 @@
     <t>EV CHARGING</t>
   </si>
   <si>
-    <t xml:space="preserve">COMPATIBLE TARIFICATOR </t>
-  </si>
-  <si>
     <t>OUI</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>9m30</t>
+  </si>
+  <si>
+    <t>COMPATIBLE</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,16 +785,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -809,10 +809,10 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -826,10 +826,10 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -843,13 +843,13 @@
         <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,10 +877,10 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
         <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -908,13 +908,13 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -928,10 +928,10 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1068,16 +1068,16 @@
         <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1091,7 +1091,7 @@
         <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="4" t="str">
         <f>"Total : " &amp;ROUND(COUNTIF(E:E,"OUI")/53*100,2) &amp; "%"</f>
@@ -1138,7 +1138,7 @@
         <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" s="4" t="str">
         <f>"Nombre incompatible : " &amp;COUNTIF(E2:E54,"NON")</f>
@@ -1157,10 +1157,10 @@
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G24" s="4" t="str">
         <f>"Total incompatible : " &amp;ROUND(COUNTIF(E:E,"NON")/53*100,2) &amp; "%"</f>
@@ -1179,7 +1179,7 @@
         <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,7 +1193,7 @@
         <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1207,10 +1207,10 @@
         <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,10 +1280,10 @@
         <v>18</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1294,10 +1294,10 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -1308,10 +1308,10 @@
         <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1322,10 +1322,10 @@
         <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1336,10 +1336,10 @@
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1350,10 +1350,10 @@
         <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1364,10 +1364,10 @@
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1378,10 +1378,10 @@
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -1392,10 +1392,10 @@
         <v>56</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -1406,10 +1406,10 @@
         <v>85</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1420,13 +1420,13 @@
         <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -1437,10 +1437,10 @@
         <v>38</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -1451,13 +1451,13 @@
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1468,13 +1468,16 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="F45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1485,10 +1488,10 @@
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -1499,10 +1502,10 @@
         <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,7 +1530,7 @@
         <v>23</v>
       </c>
       <c r="E49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,7 +1544,7 @@
         <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,7 +1558,7 @@
         <v>69</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,7 +1572,7 @@
         <v>71</v>
       </c>
       <c r="E52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,7 +1586,7 @@
         <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1600,7 @@
         <v>28</v>
       </c>
       <c r="E54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1608,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H54">
     <sortCondition ref="A2:A54"/>
   </sortState>
-  <conditionalFormatting sqref="G1:H1 G22:H22 E1:F4 E6:F1048576 E5">
+  <conditionalFormatting sqref="G1:H1 G22:H22 E1:F4 E5 E6:F1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NON">
       <formula>NOT(ISERROR(SEARCH("NON",E1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
tarificator : choix automatique du TYPM de photo / probleme famille du au fait qu'elle était au format numerique et 3 char
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66CAC91-6541-412F-A312-F0ED194D6A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A27B1-B4E0-4143-8987-8D10C940089A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="119">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t>COMPATIBLE</t>
+  </si>
+  <si>
+    <t>12s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA FAMILLE NE DOIT PAS ETRE EN NUMERIQUE </t>
   </si>
 </sst>
 </file>
@@ -759,18 +765,18 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1178,8 +1184,14 @@
       <c r="C25" t="s">
         <v>30</v>
       </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
       <c r="E25" t="s">
         <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prefix : ajout du temps d'execution du programme sur le tarif thermor et S&P
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A27B1-B4E0-4143-8987-8D10C940089A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAF3F66-0DCF-4043-8861-044CA97A2567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="121">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t xml:space="preserve">LA FAMILLE NE DOIT PAS ETRE EN NUMERIQUE </t>
+  </si>
+  <si>
+    <t>28m22</t>
+  </si>
+  <si>
+    <t>1m46</t>
   </si>
 </sst>
 </file>
@@ -765,7 +771,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F10"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1454,9 @@
       <c r="C43" t="s">
         <v>38</v>
       </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
       <c r="E43" t="s">
         <v>100</v>
       </c>
@@ -1540,6 +1549,9 @@
       </c>
       <c r="C49" t="s">
         <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>120</v>
       </c>
       <c r="E49" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
tarificator : grosse mise à jour concernant l'ajout des remises de facon automatique
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAF3F66-0DCF-4043-8861-044CA97A2567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2DE21E-A737-4A1C-B709-56CE8C1F4481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -101,9 +101,6 @@
     <t>PLANET WATTOHM</t>
   </si>
   <si>
-    <t>SCH</t>
-  </si>
-  <si>
     <t>THERMOR</t>
   </si>
   <si>
@@ -140,12 +137,6 @@
     <t>DET</t>
   </si>
   <si>
-    <t>ATOLE</t>
-  </si>
-  <si>
-    <t>ATO</t>
-  </si>
-  <si>
     <t>ALDES</t>
   </si>
   <si>
@@ -155,24 +146,12 @@
     <t>UNE</t>
   </si>
   <si>
-    <t>ARIC</t>
-  </si>
-  <si>
-    <t>ARI</t>
-  </si>
-  <si>
     <t>GEWISS</t>
   </si>
   <si>
     <t>GW</t>
   </si>
   <si>
-    <t>ORBITEC</t>
-  </si>
-  <si>
-    <t>ORB</t>
-  </si>
-  <si>
     <t>MWK</t>
   </si>
   <si>
@@ -230,12 +209,6 @@
     <t>IBO</t>
   </si>
   <si>
-    <t>LEBENOID</t>
-  </si>
-  <si>
-    <t>EBE</t>
-  </si>
-  <si>
     <t>WAGO CONTACT</t>
   </si>
   <si>
@@ -305,9 +278,6 @@
     <t>GREE</t>
   </si>
   <si>
-    <t>SCHNEIDER ELECTRIC</t>
-  </si>
-  <si>
     <t>ZEHNDER GROUP FRANCE</t>
   </si>
   <si>
@@ -341,12 +311,6 @@
     <t>OUI</t>
   </si>
   <si>
-    <t>TOTAL COMPATIBLE</t>
-  </si>
-  <si>
-    <t>NON</t>
-  </si>
-  <si>
     <t>COOPER SECURITE</t>
   </si>
   <si>
@@ -371,9 +335,6 @@
     <t>30m10</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t xml:space="preserve">COMMENTAIRE </t>
   </si>
   <si>
@@ -399,6 +360,9 @@
   </si>
   <si>
     <t>1m46</t>
+  </si>
+  <si>
+    <t>7m28</t>
   </si>
 </sst>
 </file>
@@ -768,10 +732,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,11 +746,10 @@
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,569 +760,548 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
         <v>105</v>
       </c>
-      <c r="E19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="4" t="str">
-        <f>"Total : " &amp;ROUND(COUNTIF(E:E,"OUI")/53*100,2) &amp; "%"</f>
-        <v>Total : 90,57%</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="4" t="str">
-        <f>"Nombre incompatible : " &amp;COUNTIF(E2:E54,"NON")</f>
-        <v>Nombre incompatible : 5</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="4" t="str">
-        <f>"Total incompatible : " &amp;ROUND(COUNTIF(E:E,"NON")/53*100,2) &amp; "%"</f>
-        <v>Total incompatible : 9,43%</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
@@ -1368,271 +1310,195 @@
         <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
       </c>
       <c r="E39" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>90</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E48" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C54" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A54" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H54">
-    <sortCondition ref="A2:A54"/>
+  <autoFilter ref="A1:A49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
+    <sortCondition ref="A2:A49"/>
   </sortState>
-  <conditionalFormatting sqref="G1:H1 G22:H22 E1:F4 E5 E6:F1048576">
+  <conditionalFormatting sqref="E1:F4 E5 E6:F1048576 G1 G20">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NON">
       <formula>NOT(ISERROR(SEARCH("NON",E1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
global : voir note patch 1.3 trello
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2DE21E-A737-4A1C-B709-56CE8C1F4481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DDCCF1-A754-48A9-B1BC-8AD9E5F4E11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -363,6 +363,21 @@
   </si>
   <si>
     <t>7m28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERSEN </t>
+  </si>
+  <si>
+    <t>MERSEN</t>
+  </si>
+  <si>
+    <t>FER</t>
+  </si>
+  <si>
+    <t>SCH</t>
+  </si>
+  <si>
+    <t>SCHNEIDER ELECTRIC</t>
   </si>
 </sst>
 </file>
@@ -732,10 +747,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,6 +1505,34 @@
         <v>27</v>
       </c>
       <c r="E49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mediator : ajout de la suppression des fichier image de 0ko $
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DDCCF1-A754-48A9-B1BC-8AD9E5F4E11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98470B8-6C42-4037-8741-6D5F700EAA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -749,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,13 +1260,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
         <v>90</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>90</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
         <v>90</v>
@@ -1305,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -1319,10 +1319,10 @@
         <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
         <v>90</v>
@@ -1330,13 +1330,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
         <v>90</v>
@@ -1344,16 +1344,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
         <v>90</v>
@@ -1361,33 +1358,30 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E40" t="s">
         <v>90</v>
-      </c>
-      <c r="F40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="E41" t="s">
         <v>90</v>
@@ -1395,27 +1389,33 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="D42" t="s">
+        <v>102</v>
       </c>
       <c r="E42" t="s">
         <v>90</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E43" t="s">
         <v>90</v>
@@ -1423,16 +1423,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E44" t="s">
         <v>90</v>
@@ -1440,13 +1437,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
@@ -1454,13 +1451,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
       </c>
       <c r="E46" t="s">
         <v>90</v>
@@ -1468,13 +1468,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E47" t="s">
         <v>90</v>
@@ -1482,13 +1482,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
         <v>90</v>
@@ -1496,13 +1496,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E49" t="s">
         <v>90</v>
@@ -1510,13 +1510,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
         <v>90</v>
@@ -1524,13 +1524,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="E51" t="s">
         <v>90</v>
@@ -1538,8 +1538,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
-    <sortCondition ref="A2:A49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G51">
+    <sortCondition ref="A2:A51"/>
   </sortState>
   <conditionalFormatting sqref="E1:F4 E5 E6:F1048576 G1 G20">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NON">

</xml_diff>

<commit_message>
global : ajout de nouveaux fournisseur dans les prefixes / correction nom médiator / Ajout de requetor qui permet d'ajouter la fiche technique de chaque produit et d'avoir un rendu propre sur le site
</commit_message>
<xml_diff>
--- a/PrefixeSocoda (003).xlsx
+++ b/PrefixeSocoda (003).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98470B8-6C42-4037-8741-6D5F700EAA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1198656-A0CD-4197-BB60-5DD9FEFB3863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="119">
   <si>
     <t>FABRICANT</t>
   </si>
@@ -378,6 +378,21 @@
   </si>
   <si>
     <t>SCHNEIDER ELECTRIC</t>
+  </si>
+  <si>
+    <t>19m40</t>
+  </si>
+  <si>
+    <t>ENTRELEC</t>
+  </si>
+  <si>
+    <t>TE CONNECTIVITY</t>
+  </si>
+  <si>
+    <t>pas de socoda</t>
+  </si>
+  <si>
+    <t>ENT</t>
   </si>
 </sst>
 </file>
@@ -747,10 +762,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,6 +1283,9 @@
       <c r="C33" t="s">
         <v>111</v>
       </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
       <c r="E33" t="s">
         <v>90</v>
       </c>
@@ -1423,27 +1441,27 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" t="s">
-        <v>90</v>
+        <v>118</v>
+      </c>
+      <c r="F44" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
@@ -1451,16 +1469,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
         <v>90</v>
@@ -1468,13 +1483,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>107</v>
       </c>
       <c r="E47" t="s">
         <v>90</v>
@@ -1482,13 +1500,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E48" t="s">
         <v>90</v>
@@ -1499,10 +1517,10 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
         <v>90</v>
@@ -1510,13 +1528,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
         <v>90</v>
@@ -1524,22 +1542,35 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>80</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>26</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>27</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G51">
-    <sortCondition ref="A2:A51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F52">
+    <sortCondition ref="A2:A52"/>
   </sortState>
   <conditionalFormatting sqref="E1:F4 E5 E6:F1048576 G1 G20">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NON">

</xml_diff>